<commit_message>
add some review task
</commit_message>
<xml_diff>
--- a/TO_REVIEW.XLSX
+++ b/TO_REVIEW.XLSX
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>STL</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Optimized Hashmap</t>
+  </si>
+  <si>
+    <t>Problem 17</t>
+  </si>
+  <si>
+    <t>string initlialization</t>
   </si>
 </sst>
 </file>
@@ -366,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F5"/>
+  <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,6 +420,16 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update 0226, Add red black tree in TO_REVIEW
</commit_message>
<xml_diff>
--- a/TO_REVIEW.XLSX
+++ b/TO_REVIEW.XLSX
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>STL</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>string initlialization</t>
+  </si>
+  <si>
+    <t>Red Black Tree</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
   <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +398,9 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>